<commit_message>
all fine in master
</commit_message>
<xml_diff>
--- a/Results/table_params.xlsx
+++ b/Results/table_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbueren\Google Drive\overdrilling\fortran\Unobs_heterogeneity_ME\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF7F6AE1-FD60-48CD-85A4-B7EF60FBE437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0E334B-746D-45E8-A0E5-5DF6136D7064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4CBDE4B8-43E2-4423-B618-528CE52FA05F}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="2" xr2:uid="{4CBDE4B8-43E2-4423-B618-528CE52FA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6993,7 +6993,7 @@
   <dimension ref="E7:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7077,49 +7077,49 @@
     </row>
     <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <v>0.9</v>
       </c>
       <c r="G10">
-        <v>11.5</v>
-      </c>
-      <c r="H10" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>27.2</v>
+      </c>
+      <c r="H10">
+        <v>0.99990000000000001</v>
       </c>
       <c r="I10">
-        <v>0.04</v>
+        <f>1-H10</f>
+        <v>9.9999999999988987E-5</v>
       </c>
       <c r="J10" t="s">
         <v>18</v>
       </c>
       <c r="K10" s="1">
-        <v>1733</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="11" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <v>0.9</v>
       </c>
       <c r="G11">
-        <v>27.2</v>
-      </c>
-      <c r="H11">
-        <v>0.99990000000000001</v>
+        <v>11.5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I11">
-        <f>1-H11</f>
-        <v>9.9999999999988987E-5</v>
+        <v>0.04</v>
       </c>
       <c r="J11" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="1">
-        <v>2306</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>